<commit_message>
heb xls sheet 2 toegevoegd
</commit_message>
<xml_diff>
--- a/BUDATA_DWH.xlsx
+++ b/BUDATA_DWH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="240">
   <si>
     <t>Context</t>
   </si>
@@ -736,6 +736,9 @@
   </si>
   <si>
     <t>Dubbel</t>
+  </si>
+  <si>
+    <t>sheet 2 ter test</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1089,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
@@ -3643,10 +3646,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
eerste deel mapping herkomst uit BUTOPO/GPCARTO/Overig
</commit_message>
<xml_diff>
--- a/BUDATA_DWH.xlsx
+++ b/BUDATA_DWH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="12525" windowHeight="9765"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="251">
   <si>
     <t>Context</t>
   </si>
@@ -742,6 +742,36 @@
   </si>
   <si>
     <t>En nog een wijziging om te testen</t>
+  </si>
+  <si>
+    <t>Herkomst</t>
+  </si>
+  <si>
+    <t>BUTOPO</t>
+  </si>
+  <si>
+    <t>BUTOPO/GPCARTO</t>
+  </si>
+  <si>
+    <t>Opmerking</t>
+  </si>
+  <si>
+    <t>niet compleet</t>
+  </si>
+  <si>
+    <t>leeg</t>
+  </si>
+  <si>
+    <t>BUDATA</t>
+  </si>
+  <si>
+    <t>te verwijderen?</t>
+  </si>
+  <si>
+    <t>GPCARTO</t>
+  </si>
+  <si>
+    <t>Gisib</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1122,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,9 +1131,11 @@
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +1145,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1124,8 +1162,11 @@
       <c r="C2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1177,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1188,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1199,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1221,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1232,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1202,7 +1243,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1213,7 +1254,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1224,7 +1265,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1279,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1290,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1301,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1271,7 +1312,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1323,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1293,7 +1334,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1304,7 +1345,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1315,7 +1356,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1367,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1337,7 +1378,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1348,7 +1389,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1359,7 +1400,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1370,7 +1411,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1422,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1433,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1403,7 +1444,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1413,8 +1454,11 @@
       <c r="C28" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1425,7 +1469,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1436,7 +1480,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1447,7 +1491,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1458,7 +1502,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1469,7 +1513,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1480,7 +1524,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1491,7 +1535,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1501,8 +1545,11 @@
       <c r="C36" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1513,7 +1560,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1571,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1535,7 +1582,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1545,8 +1592,11 @@
       <c r="C40" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1557,7 +1607,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1567,8 +1617,11 @@
       <c r="C42" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1632,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1589,8 +1642,11 @@
       <c r="C44" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1601,7 +1657,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1612,7 +1668,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1623,7 +1679,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1634,7 +1690,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1701,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1659,7 +1715,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1669,8 +1725,11 @@
       <c r="C51" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1681,7 +1740,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1751,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1762,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1713,8 +1772,11 @@
       <c r="C55" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1787,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1735,8 +1797,11 @@
       <c r="C57" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1746,6 +1811,9 @@
       <c r="C58" t="s">
         <v>229</v>
       </c>
+      <c r="D58" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1758,7 +1826,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1769,7 +1837,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1780,7 +1848,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1791,7 +1859,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1870,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1813,7 +1881,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1824,7 +1892,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +1903,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -1846,7 +1914,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1925,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -1867,8 +1935,11 @@
       <c r="C69" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -1879,7 +1950,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -1901,7 +1972,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1986,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1997,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -1936,8 +2007,11 @@
       <c r="C75" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -1947,8 +2021,11 @@
       <c r="C76" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -1958,8 +2035,11 @@
       <c r="C77" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -1969,8 +2049,11 @@
       <c r="C78" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -1981,7 +2064,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -1991,8 +2074,11 @@
       <c r="C80" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2003,7 +2089,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2014,7 +2100,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +2111,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2036,7 +2122,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2047,7 +2133,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2144,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2069,7 +2155,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2080,7 +2166,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2177,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +2188,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2113,7 +2199,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2124,7 +2210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2135,7 +2221,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2145,8 +2231,11 @@
       <c r="C94" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2157,7 +2246,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -2167,8 +2256,11 @@
       <c r="C96" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -2178,8 +2270,11 @@
       <c r="C97" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -2193,7 +2288,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -2203,8 +2298,11 @@
       <c r="C99" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -2214,8 +2312,11 @@
       <c r="C100" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -2226,7 +2327,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -2236,8 +2337,11 @@
       <c r="C102" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -2247,8 +2351,14 @@
       <c r="C103" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>242</v>
+      </c>
+      <c r="E103" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -2258,8 +2368,11 @@
       <c r="C104" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -2269,8 +2382,11 @@
       <c r="C105" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -2280,8 +2396,11 @@
       <c r="C106" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -2290,6 +2409,9 @@
       </c>
       <c r="C107" t="s">
         <v>229</v>
+      </c>
+      <c r="D107" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2303,7 +2425,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -2313,8 +2435,11 @@
       <c r="C109" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -2324,8 +2449,11 @@
       <c r="C110" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -2335,8 +2463,11 @@
       <c r="C111" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -2346,8 +2477,11 @@
       <c r="C112" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -2358,7 +2492,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -2369,7 +2503,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -2379,8 +2513,11 @@
       <c r="C115" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -2390,8 +2527,11 @@
       <c r="C116" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -2402,7 +2542,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -2413,7 +2553,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -2427,7 +2567,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -2438,7 +2578,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -2449,7 +2589,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -2460,7 +2600,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -2471,7 +2611,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -2482,7 +2622,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -2493,7 +2633,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -2504,7 +2644,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -2515,7 +2655,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -2526,7 +2666,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2677,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -2548,7 +2688,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -2559,7 +2699,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -2570,7 +2710,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -2581,7 +2721,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -2592,7 +2732,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -2602,8 +2742,11 @@
       <c r="C135" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -2613,8 +2756,11 @@
       <c r="C136" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -2624,8 +2770,11 @@
       <c r="C137" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -2636,7 +2785,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -2647,7 +2796,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -2658,7 +2807,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -2668,8 +2817,11 @@
       <c r="C141" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -2680,7 +2832,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -2690,8 +2842,11 @@
       <c r="C143" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -2701,8 +2856,11 @@
       <c r="C144" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -2713,7 +2871,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -2724,7 +2882,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -2734,8 +2892,11 @@
       <c r="C147" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -2745,8 +2906,11 @@
       <c r="C148" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -2756,8 +2920,11 @@
       <c r="C149" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -2767,8 +2934,11 @@
       <c r="C150" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -2778,8 +2948,11 @@
       <c r="C151" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -2789,8 +2962,11 @@
       <c r="C152" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -2801,7 +2977,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -2812,7 +2988,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -2822,8 +2998,11 @@
       <c r="C155" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E155" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -2834,7 +3013,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -2845,7 +3024,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -2855,8 +3034,11 @@
       <c r="C158" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -2866,8 +3048,11 @@
       <c r="C159" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>9</v>
       </c>
@@ -2878,7 +3063,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -2888,8 +3073,11 @@
       <c r="C161" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -2899,8 +3087,11 @@
       <c r="C162" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E162" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -2911,7 +3102,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -2922,7 +3113,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -2933,7 +3124,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>9</v>
       </c>
@@ -2944,7 +3135,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -2955,7 +3146,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -2966,7 +3157,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -2977,7 +3168,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -2988,7 +3179,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -2998,8 +3189,11 @@
       <c r="C171" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E171" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -3009,8 +3203,11 @@
       <c r="C172" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -3021,7 +3218,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -3032,7 +3229,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -3042,8 +3239,11 @@
       <c r="C175" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>9</v>
       </c>
@@ -3053,8 +3253,11 @@
       <c r="C176" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -3065,7 +3268,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>5</v>
       </c>
@@ -3075,8 +3278,11 @@
       <c r="C178" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E178" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>5</v>
       </c>
@@ -3087,7 +3293,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3304,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>5</v>
       </c>
@@ -3108,8 +3314,11 @@
       <c r="C181" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E181" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -3120,7 +3329,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>5</v>
       </c>
@@ -3130,8 +3339,11 @@
       <c r="C183" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>5</v>
       </c>
@@ -3142,7 +3354,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>5</v>
       </c>
@@ -3153,7 +3365,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>5</v>
       </c>
@@ -3163,8 +3375,11 @@
       <c r="C186" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E186" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>5</v>
       </c>
@@ -3175,7 +3390,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>5</v>
       </c>
@@ -3186,7 +3401,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>5</v>
       </c>
@@ -3196,8 +3411,11 @@
       <c r="C189" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E189" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>5</v>
       </c>
@@ -3208,7 +3426,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>5</v>
       </c>
@@ -3219,7 +3437,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>5</v>
       </c>
@@ -3229,8 +3447,11 @@
       <c r="C192" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E192" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>5</v>
       </c>
@@ -3241,7 +3462,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>5</v>
       </c>
@@ -3251,8 +3472,11 @@
       <c r="C194" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>5</v>
       </c>
@@ -3263,7 +3487,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>5</v>
       </c>
@@ -3277,7 +3501,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>5</v>
       </c>
@@ -3288,7 +3512,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>5</v>
       </c>
@@ -3299,7 +3523,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>5</v>
       </c>
@@ -3310,7 +3534,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>5</v>
       </c>
@@ -3321,7 +3545,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>5</v>
       </c>
@@ -3332,7 +3556,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>5</v>
       </c>
@@ -3354,7 +3578,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>5</v>
       </c>
@@ -3365,7 +3589,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>5</v>
       </c>
@@ -3376,7 +3600,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>5</v>
       </c>
@@ -3387,7 +3611,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>5</v>
       </c>
@@ -3397,8 +3621,11 @@
       <c r="C207" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D207" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>3</v>
       </c>
@@ -3407,6 +3634,9 @@
       </c>
       <c r="C208" t="s">
         <v>229</v>
+      </c>
+      <c r="D208" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -3420,7 +3650,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>3</v>
       </c>
@@ -3431,7 +3661,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>3</v>
       </c>
@@ -3442,7 +3672,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>3</v>
       </c>
@@ -3453,7 +3683,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>3</v>
       </c>
@@ -3464,7 +3694,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>3</v>
       </c>
@@ -3474,8 +3704,11 @@
       <c r="C214" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D214" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>3</v>
       </c>
@@ -3486,7 +3719,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>3</v>
       </c>
@@ -3497,7 +3730,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>3</v>
       </c>
@@ -3508,7 +3741,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>3</v>
       </c>
@@ -3522,7 +3755,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>3</v>
       </c>
@@ -3533,7 +3766,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>3</v>
       </c>
@@ -3555,7 +3788,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>3</v>
       </c>
@@ -3565,8 +3798,11 @@
       <c r="C222" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D222" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>3</v>
       </c>
@@ -3577,7 +3813,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>3</v>
       </c>
@@ -3588,7 +3824,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>3</v>
       </c>
@@ -3599,7 +3835,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>3</v>
       </c>
@@ -3609,8 +3845,11 @@
       <c r="C226" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>3</v>
       </c>
@@ -3620,8 +3859,11 @@
       <c r="C227" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D227" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>3</v>
       </c>
@@ -3636,7 +3878,7 @@
   <autoFilter ref="A1:C228">
     <filterColumn colId="2">
       <filters>
-        <filter val="Basisobject"/>
+        <filter val="Beheerobject"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3649,11 +3891,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>